<commit_message>
added diagram of iterations and removed old file
</commit_message>
<xml_diff>
--- a/FVisual_Documentation/Projekttagebuch.xlsx
+++ b/FVisual_Documentation/Projekttagebuch.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\syp_pos_dbi\FVisual\FVisual_Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE726CE6-8E99-46FA-825E-811CF964DA07}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BA42754-B16E-484C-BE08-7B0D13DBB7F1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13425" firstSheet="1" activeTab="4" xr2:uid="{D18071EC-83FE-4EFA-8D7C-A4670CF93F56}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13425" firstSheet="2" activeTab="5" xr2:uid="{D18071EC-83FE-4EFA-8D7C-A4670CF93F56}"/>
   </bookViews>
   <sheets>
     <sheet name="Übersicht Tag" sheetId="4" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="MO 30.09.2019 - SYP1" sheetId="1" r:id="rId3"/>
     <sheet name="MO 03.10.2019 - WINF" sheetId="6" r:id="rId4"/>
     <sheet name="MO 07.10.2019 - SYP1" sheetId="8" r:id="rId5"/>
+    <sheet name="MO 14.10.2019 - SYP1" sheetId="9" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="60">
   <si>
     <t>In Bearbeitung</t>
   </si>
@@ -212,6 +213,9 @@
   </si>
   <si>
     <t>Person(en)</t>
+  </si>
+  <si>
+    <t>MO. / 07.10.2019</t>
   </si>
 </sst>
 </file>
@@ -353,7 +357,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -434,23 +438,29 @@
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1012,10 +1022,10 @@
       <c r="B2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="34" t="s">
+      <c r="C2" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="34"/>
+      <c r="D2" s="32"/>
       <c r="E2" s="1" t="s">
         <v>17</v>
       </c>
@@ -1041,10 +1051,10 @@
     </row>
     <row r="4" spans="1:6" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B4" s="16"/>
-      <c r="C4" s="35" t="s">
+      <c r="C4" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="35"/>
+      <c r="D4" s="34"/>
       <c r="E4" s="19">
         <v>100</v>
       </c>
@@ -1054,10 +1064,10 @@
     </row>
     <row r="5" spans="1:6" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B5" s="16"/>
-      <c r="C5" s="31" t="s">
+      <c r="C5" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="31"/>
+      <c r="D5" s="35"/>
       <c r="E5" s="21">
         <v>100</v>
       </c>
@@ -1067,10 +1077,10 @@
     </row>
     <row r="6" spans="1:6" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B6" s="16"/>
-      <c r="C6" s="32" t="s">
+      <c r="C6" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="32"/>
+      <c r="D6" s="36"/>
       <c r="E6" s="23">
         <v>100</v>
       </c>
@@ -1082,10 +1092,10 @@
       <c r="B7" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="31" t="s">
+      <c r="C7" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="31"/>
+      <c r="D7" s="35"/>
       <c r="E7" s="21">
         <v>50</v>
       </c>
@@ -1095,10 +1105,10 @@
     </row>
     <row r="8" spans="1:6" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B8" s="16"/>
-      <c r="C8" s="32" t="s">
+      <c r="C8" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="32"/>
+      <c r="D8" s="36"/>
       <c r="E8" s="23">
         <v>70</v>
       </c>
@@ -1108,10 +1118,10 @@
     </row>
     <row r="9" spans="1:6" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B9" s="16"/>
-      <c r="C9" s="32" t="s">
+      <c r="C9" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="32"/>
+      <c r="D9" s="36"/>
       <c r="E9" s="23">
         <v>15</v>
       </c>
@@ -1121,10 +1131,10 @@
     </row>
     <row r="10" spans="1:6" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B10" s="16"/>
-      <c r="C10" s="32" t="s">
+      <c r="C10" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="D10" s="32"/>
+      <c r="D10" s="36"/>
       <c r="E10" s="23">
         <v>20</v>
       </c>
@@ -1147,103 +1157,103 @@
     </row>
     <row r="12" spans="1:6" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B12" s="16"/>
-      <c r="C12" s="30"/>
-      <c r="D12" s="30"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="37"/>
     </row>
     <row r="13" spans="1:6" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B13" s="16"/>
-      <c r="C13" s="30"/>
-      <c r="D13" s="30"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="37"/>
     </row>
     <row r="14" spans="1:6" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B14" s="16"/>
-      <c r="C14" s="30"/>
-      <c r="D14" s="30"/>
+      <c r="C14" s="37"/>
+      <c r="D14" s="37"/>
     </row>
     <row r="15" spans="1:6" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B15" s="16"/>
-      <c r="C15" s="30"/>
-      <c r="D15" s="30"/>
+      <c r="C15" s="37"/>
+      <c r="D15" s="37"/>
     </row>
     <row r="16" spans="1:6" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B16" s="16"/>
-      <c r="C16" s="30"/>
-      <c r="D16" s="30"/>
+      <c r="C16" s="37"/>
+      <c r="D16" s="37"/>
     </row>
     <row r="17" spans="2:4" ht="15" x14ac:dyDescent="0.45">
       <c r="B17" s="16"/>
-      <c r="C17" s="30"/>
-      <c r="D17" s="30"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="37"/>
     </row>
     <row r="18" spans="2:4" ht="15" x14ac:dyDescent="0.45">
       <c r="B18" s="16"/>
-      <c r="C18" s="30"/>
-      <c r="D18" s="30"/>
+      <c r="C18" s="37"/>
+      <c r="D18" s="37"/>
     </row>
     <row r="19" spans="2:4" ht="15" x14ac:dyDescent="0.45">
       <c r="B19" s="16"/>
-      <c r="C19" s="30"/>
-      <c r="D19" s="30"/>
+      <c r="C19" s="37"/>
+      <c r="D19" s="37"/>
     </row>
     <row r="20" spans="2:4" ht="15" x14ac:dyDescent="0.45">
       <c r="B20" s="16"/>
-      <c r="C20" s="30"/>
-      <c r="D20" s="30"/>
+      <c r="C20" s="37"/>
+      <c r="D20" s="37"/>
     </row>
     <row r="21" spans="2:4" ht="15" x14ac:dyDescent="0.45">
       <c r="B21" s="16"/>
-      <c r="C21" s="30"/>
-      <c r="D21" s="30"/>
+      <c r="C21" s="37"/>
+      <c r="D21" s="37"/>
     </row>
     <row r="22" spans="2:4" ht="15" x14ac:dyDescent="0.45">
       <c r="B22" s="16"/>
-      <c r="C22" s="30"/>
-      <c r="D22" s="30"/>
+      <c r="C22" s="37"/>
+      <c r="D22" s="37"/>
     </row>
     <row r="23" spans="2:4" ht="15" x14ac:dyDescent="0.45">
       <c r="B23" s="16"/>
-      <c r="C23" s="30"/>
-      <c r="D23" s="30"/>
+      <c r="C23" s="37"/>
+      <c r="D23" s="37"/>
     </row>
     <row r="24" spans="2:4" ht="15" x14ac:dyDescent="0.45">
       <c r="B24" s="16"/>
-      <c r="C24" s="30"/>
-      <c r="D24" s="30"/>
+      <c r="C24" s="37"/>
+      <c r="D24" s="37"/>
     </row>
     <row r="25" spans="2:4" ht="15" x14ac:dyDescent="0.45">
       <c r="B25" s="16"/>
-      <c r="C25" s="30"/>
-      <c r="D25" s="30"/>
+      <c r="C25" s="37"/>
+      <c r="D25" s="37"/>
     </row>
     <row r="26" spans="2:4" ht="15" x14ac:dyDescent="0.45">
       <c r="B26" s="16"/>
-      <c r="C26" s="30"/>
-      <c r="D26" s="30"/>
+      <c r="C26" s="37"/>
+      <c r="D26" s="37"/>
     </row>
     <row r="27" spans="2:4" ht="15" x14ac:dyDescent="0.45">
       <c r="B27" s="16"/>
-      <c r="C27" s="30"/>
-      <c r="D27" s="30"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
     </row>
     <row r="28" spans="2:4" ht="15" x14ac:dyDescent="0.45">
       <c r="B28" s="16"/>
-      <c r="C28" s="30"/>
-      <c r="D28" s="30"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="37"/>
     </row>
     <row r="29" spans="2:4" ht="15" x14ac:dyDescent="0.45">
       <c r="B29" s="16"/>
-      <c r="C29" s="30"/>
-      <c r="D29" s="30"/>
+      <c r="C29" s="37"/>
+      <c r="D29" s="37"/>
     </row>
     <row r="30" spans="2:4" ht="15" x14ac:dyDescent="0.45">
       <c r="B30" s="16"/>
-      <c r="C30" s="30"/>
-      <c r="D30" s="30"/>
+      <c r="C30" s="37"/>
+      <c r="D30" s="37"/>
     </row>
     <row r="31" spans="2:4" ht="15" x14ac:dyDescent="0.45">
       <c r="B31" s="16"/>
-      <c r="C31" s="30"/>
-      <c r="D31" s="30"/>
+      <c r="C31" s="37"/>
+      <c r="D31" s="37"/>
     </row>
     <row r="32" spans="2:4" ht="15" x14ac:dyDescent="0.45">
       <c r="B32" s="16"/>
@@ -1265,36 +1275,36 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C8:D8"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C31:D31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1324,10 +1334,10 @@
       <c r="B2" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="36"/>
+      <c r="D2" s="38"/>
       <c r="E2" s="8" t="s">
         <v>8</v>
       </c>
@@ -1342,10 +1352,10 @@
       <c r="B3" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="37" t="s">
+      <c r="C3" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="37"/>
+      <c r="D3" s="39"/>
       <c r="E3" s="12" t="s">
         <v>29</v>
       </c>
@@ -1416,9 +1426,9 @@
       <c r="G11" s="4"/>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="C12" s="30"/>
-      <c r="D12" s="30"/>
-      <c r="E12" s="30"/>
+      <c r="C12" s="37"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="37"/>
     </row>
     <row r="13" spans="2:7" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="8" t="s">
@@ -1557,10 +1567,10 @@
       <c r="B2" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="36"/>
+      <c r="D2" s="38"/>
       <c r="E2" s="10" t="s">
         <v>8</v>
       </c>
@@ -1575,10 +1585,10 @@
       <c r="B3" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="37" t="s">
+      <c r="C3" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="37"/>
+      <c r="D3" s="39"/>
       <c r="E3" s="15" t="s">
         <v>29</v>
       </c>
@@ -1828,8 +1838,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8FC4F49-D022-4F6F-A786-75A55A7C7901}">
   <dimension ref="B2:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView zoomScale="83" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1848,10 +1858,10 @@
       <c r="B2" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="36"/>
+      <c r="D2" s="38"/>
       <c r="E2" s="28" t="s">
         <v>8</v>
       </c>
@@ -1864,12 +1874,12 @@
     </row>
     <row r="3" spans="2:7" s="14" customFormat="1" ht="21.4" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B3" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="C3" s="37" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="37"/>
+      <c r="D3" s="39"/>
       <c r="E3" s="29" t="s">
         <v>29</v>
       </c>
@@ -2091,6 +2101,294 @@
         <v>5</v>
       </c>
       <c r="D24" s="28" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" s="14" customFormat="1" ht="21.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+    </row>
+    <row r="26" spans="2:7" s="14" customFormat="1" ht="21.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02EA03C1-25CA-42A6-9B2D-CB7F8E650248}">
+  <dimension ref="B2:G26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="2.86328125" customWidth="1"/>
+    <col min="2" max="2" width="56.1328125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="34.265625" customWidth="1"/>
+    <col min="4" max="4" width="31.86328125" customWidth="1"/>
+    <col min="5" max="5" width="27" customWidth="1"/>
+    <col min="6" max="6" width="29.3984375" customWidth="1"/>
+    <col min="7" max="7" width="28.73046875" customWidth="1"/>
+    <col min="8" max="8" width="18.59765625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="38"/>
+      <c r="E2" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="30" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" s="14" customFormat="1" ht="21.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B3" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="30" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" s="14" customFormat="1" ht="21.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B6" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="31">
+        <v>50</v>
+      </c>
+      <c r="D6" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+    </row>
+    <row r="7" spans="2:7" s="14" customFormat="1" ht="21.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B7" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" s="31">
+        <v>30</v>
+      </c>
+      <c r="D7" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+    </row>
+    <row r="8" spans="2:7" s="14" customFormat="1" ht="21.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B8" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" s="31">
+        <v>15</v>
+      </c>
+      <c r="D8" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="31" t="s">
+        <v>51</v>
+      </c>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+    </row>
+    <row r="9" spans="2:7" s="2" customFormat="1" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B9" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="31">
+        <v>30</v>
+      </c>
+      <c r="D9" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="E9" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+    </row>
+    <row r="11" spans="2:7" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" s="30" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" s="30" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" s="14" customFormat="1" ht="21.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B12" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="31">
+        <v>50</v>
+      </c>
+      <c r="E12" s="31">
+        <v>100</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" s="14" customFormat="1" ht="21.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B13" s="31"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+    </row>
+    <row r="15" spans="2:7" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="F15" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="G15" s="30" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" s="14" customFormat="1" ht="21.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B16" s="31"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+    </row>
+    <row r="17" spans="2:7" s="14" customFormat="1" ht="21.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B17" s="31"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+    </row>
+    <row r="18" spans="2:7" s="14" customFormat="1" ht="21.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B18" s="31"/>
+      <c r="C18" s="31"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+    </row>
+    <row r="20" spans="2:7" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" s="30" t="s">
+        <v>58</v>
+      </c>
+      <c r="D20" s="30" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" s="14" customFormat="1" ht="21.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B21" s="13"/>
+      <c r="C21" s="31"/>
+      <c r="D21" s="31"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+    </row>
+    <row r="22" spans="2:7" s="14" customFormat="1" ht="21.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B22" s="13"/>
+      <c r="C22" s="31"/>
+      <c r="D22" s="31"/>
+      <c r="E22" s="31"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
+    </row>
+    <row r="24" spans="2:7" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" s="30" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" s="30" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
basic rest; stuetzpunkt advanced rest; update Projekttabebuch
</commit_message>
<xml_diff>
--- a/FVisual_Documentation/Projekttagebuch.xlsx
+++ b/FVisual_Documentation/Projekttagebuch.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\syp_pos_dbi\FVisual\FVisual_Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75C5DDB0-4E41-499B-B99F-DD947C65746F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FDCF922-69B0-41DF-AFCF-6F6E4752C68D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13425" activeTab="7" xr2:uid="{D18071EC-83FE-4EFA-8D7C-A4670CF93F56}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13425" activeTab="8" xr2:uid="{D18071EC-83FE-4EFA-8D7C-A4670CF93F56}"/>
   </bookViews>
   <sheets>
     <sheet name="Übersicht Tag" sheetId="4" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="14.10." sheetId="9" r:id="rId6"/>
     <sheet name="15.10." sheetId="11" r:id="rId7"/>
     <sheet name="21.10." sheetId="13" r:id="rId8"/>
+    <sheet name="22.10." sheetId="15" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="93">
   <si>
     <t>In Bearbeitung</t>
   </si>
@@ -275,6 +276,48 @@
   </si>
   <si>
     <t>Di. / 03.10.2019</t>
+  </si>
+  <si>
+    <t>Di. / 22.10.2019</t>
+  </si>
+  <si>
+    <t>Implementierung WS &amp; BLL</t>
+  </si>
+  <si>
+    <t>Erstellung Login GUI</t>
+  </si>
+  <si>
+    <t>Erstellung Basic REST</t>
+  </si>
+  <si>
+    <t>Erstellung Stuetzpunkt REST</t>
+  </si>
+  <si>
+    <t>Erstellung Basic&amp;Stuetzpunkt parser</t>
+  </si>
+  <si>
+    <t>Erstellung default handlers</t>
+  </si>
+  <si>
+    <t>Erstellung security w/o DB Check</t>
+  </si>
+  <si>
+    <t>Erstellung BLL JavaFX</t>
+  </si>
+  <si>
+    <t>Erstellung Stuetzpunkt Advanced REST</t>
+  </si>
+  <si>
+    <t>Beschreibung von User Stories</t>
+  </si>
+  <si>
+    <t>Implementierung Maps Android</t>
+  </si>
+  <si>
+    <t>Erstellung Admin-GUI</t>
+  </si>
+  <si>
+    <t>Erstellung Stuetzpunktverwaltung JavaFx</t>
   </si>
 </sst>
 </file>
@@ -416,7 +459,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -506,24 +549,6 @@
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -531,6 +556,30 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -850,7 +899,7 @@
   <dimension ref="B1:G21"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -895,10 +944,10 @@
       <c r="D3" s="26">
         <v>100</v>
       </c>
-      <c r="E3" s="41" t="s">
+      <c r="E3" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="41" t="s">
+      <c r="F3" s="35" t="s">
         <v>29</v>
       </c>
       <c r="G3" s="25" t="s">
@@ -1005,11 +1054,21 @@
     </row>
     <row r="9" spans="2:7" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B9" s="25"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="25"/>
+      <c r="C9" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="26">
+        <v>100</v>
+      </c>
+      <c r="E9" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="F9" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" s="25" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="10" spans="2:7" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B10" s="25"/>
@@ -1116,8 +1175,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A64AB570-BFC1-4B04-BC88-2752E218D317}">
   <dimension ref="A2:H37"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20:D20"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1133,10 +1192,10 @@
       <c r="B2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="37" t="s">
+      <c r="C2" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="37"/>
+      <c r="D2" s="41"/>
       <c r="E2" s="1" t="s">
         <v>17</v>
       </c>
@@ -1149,10 +1208,10 @@
       <c r="B3" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="36"/>
+      <c r="D3" s="38"/>
       <c r="E3" s="17">
         <v>100</v>
       </c>
@@ -1162,10 +1221,10 @@
     </row>
     <row r="4" spans="1:8" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B4" s="16"/>
-      <c r="C4" s="38" t="s">
+      <c r="C4" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="38"/>
+      <c r="D4" s="40"/>
       <c r="E4" s="19">
         <v>100</v>
       </c>
@@ -1175,10 +1234,10 @@
     </row>
     <row r="5" spans="1:8" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B5" s="16"/>
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="34"/>
+      <c r="D5" s="37"/>
       <c r="E5" s="21">
         <v>100</v>
       </c>
@@ -1188,10 +1247,10 @@
     </row>
     <row r="6" spans="1:8" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B6" s="16"/>
-      <c r="C6" s="35" t="s">
+      <c r="C6" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="35"/>
+      <c r="D6" s="36"/>
       <c r="E6" s="23">
         <v>100</v>
       </c>
@@ -1203,10 +1262,10 @@
       <c r="B7" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="34" t="s">
+      <c r="C7" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="34"/>
+      <c r="D7" s="37"/>
       <c r="E7" s="21">
         <v>50</v>
       </c>
@@ -1216,10 +1275,10 @@
     </row>
     <row r="8" spans="1:8" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B8" s="16"/>
-      <c r="C8" s="35" t="s">
+      <c r="C8" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="35"/>
+      <c r="D8" s="36"/>
       <c r="E8" s="23">
         <v>70</v>
       </c>
@@ -1229,10 +1288,10 @@
     </row>
     <row r="9" spans="1:8" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B9" s="16"/>
-      <c r="C9" s="35" t="s">
+      <c r="C9" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="35"/>
+      <c r="D9" s="36"/>
       <c r="E9" s="23">
         <v>15</v>
       </c>
@@ -1242,10 +1301,10 @@
     </row>
     <row r="10" spans="1:8" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B10" s="16"/>
-      <c r="C10" s="35" t="s">
+      <c r="C10" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="D10" s="35"/>
+      <c r="D10" s="36"/>
       <c r="E10" s="23">
         <v>20</v>
       </c>
@@ -1255,10 +1314,10 @@
     </row>
     <row r="11" spans="1:8" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B11" s="16"/>
-      <c r="C11" s="36" t="s">
+      <c r="C11" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="D11" s="36"/>
+      <c r="D11" s="38"/>
       <c r="E11" s="17">
         <v>80</v>
       </c>
@@ -1270,10 +1329,10 @@
       <c r="B12" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="C12" s="34" t="s">
+      <c r="C12" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="D12" s="34"/>
+      <c r="D12" s="37"/>
       <c r="E12" s="21">
         <v>70</v>
       </c>
@@ -1284,10 +1343,10 @@
     </row>
     <row r="13" spans="1:8" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B13" s="16"/>
-      <c r="C13" s="35" t="s">
+      <c r="C13" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="D13" s="35"/>
+      <c r="D13" s="36"/>
       <c r="E13" s="23">
         <v>50</v>
       </c>
@@ -1298,10 +1357,10 @@
     </row>
     <row r="14" spans="1:8" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B14" s="16"/>
-      <c r="C14" s="36" t="s">
+      <c r="C14" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="D14" s="36"/>
+      <c r="D14" s="38"/>
       <c r="E14" s="17">
         <v>30</v>
       </c>
@@ -1312,10 +1371,10 @@
     </row>
     <row r="15" spans="1:8" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B15" s="16"/>
-      <c r="C15" s="36" t="s">
+      <c r="C15" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="D15" s="36"/>
+      <c r="D15" s="38"/>
       <c r="E15" s="17">
         <v>15</v>
       </c>
@@ -1326,10 +1385,10 @@
     </row>
     <row r="16" spans="1:8" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B16" s="16"/>
-      <c r="C16" s="38" t="s">
+      <c r="C16" s="40" t="s">
         <v>54</v>
       </c>
-      <c r="D16" s="38"/>
+      <c r="D16" s="40"/>
       <c r="E16" s="19">
         <v>30</v>
       </c>
@@ -1338,12 +1397,12 @@
       </c>
       <c r="H16" s="32"/>
     </row>
-    <row r="17" spans="2:6" ht="15" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:8" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B17" s="16"/>
-      <c r="C17" s="34" t="s">
+      <c r="C17" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="D17" s="34"/>
+      <c r="D17" s="37"/>
       <c r="E17" s="21">
         <v>30</v>
       </c>
@@ -1351,14 +1410,14 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="2:6" ht="15" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:8" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B18" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="C18" s="35" t="s">
+      <c r="C18" s="36" t="s">
         <v>73</v>
       </c>
-      <c r="D18" s="35"/>
+      <c r="D18" s="36"/>
       <c r="E18" s="23">
         <v>140</v>
       </c>
@@ -1366,72 +1425,156 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="2:6" ht="15" x14ac:dyDescent="0.45">
-      <c r="B19" s="16"/>
-      <c r="C19" s="33"/>
-      <c r="D19" s="33"/>
-    </row>
-    <row r="20" spans="2:6" ht="15" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:8" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B19" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="C19" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="D19" s="36"/>
+      <c r="E19" s="23">
+        <v>40</v>
+      </c>
+      <c r="F19" s="24" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B20" s="16"/>
-      <c r="C20" s="33"/>
-      <c r="D20" s="33"/>
-    </row>
-    <row r="21" spans="2:6" ht="15" x14ac:dyDescent="0.45">
+      <c r="C20" s="37" t="s">
+        <v>89</v>
+      </c>
+      <c r="D20" s="37"/>
+      <c r="E20" s="21">
+        <v>110</v>
+      </c>
+      <c r="F20" s="22" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B21" s="16"/>
-      <c r="C21" s="33"/>
-      <c r="D21" s="33"/>
-    </row>
-    <row r="22" spans="2:6" ht="15" x14ac:dyDescent="0.45">
+      <c r="C21" s="36" t="s">
+        <v>72</v>
+      </c>
+      <c r="D21" s="36"/>
+      <c r="E21" s="23">
+        <v>270</v>
+      </c>
+      <c r="F21" s="24" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B22" s="16"/>
-      <c r="C22" s="33"/>
-      <c r="D22" s="33"/>
-    </row>
-    <row r="23" spans="2:6" ht="15" x14ac:dyDescent="0.45">
+      <c r="C22" s="36" t="s">
+        <v>84</v>
+      </c>
+      <c r="D22" s="36"/>
+      <c r="E22" s="23">
+        <v>50</v>
+      </c>
+      <c r="F22" s="24" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B23" s="16"/>
-      <c r="C23" s="33"/>
-      <c r="D23" s="33"/>
-    </row>
-    <row r="24" spans="2:6" ht="15" x14ac:dyDescent="0.45">
+      <c r="C23" s="36" t="s">
+        <v>85</v>
+      </c>
+      <c r="D23" s="36"/>
+      <c r="E23" s="23">
+        <v>300</v>
+      </c>
+      <c r="F23" s="24" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B24" s="16"/>
-      <c r="C24" s="33"/>
-      <c r="D24" s="33"/>
-    </row>
-    <row r="25" spans="2:6" ht="15" x14ac:dyDescent="0.45">
+      <c r="C24" s="36" t="s">
+        <v>86</v>
+      </c>
+      <c r="D24" s="36"/>
+      <c r="E24" s="23">
+        <v>20</v>
+      </c>
+      <c r="F24" s="24" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B25" s="16"/>
-      <c r="C25" s="33"/>
-      <c r="D25" s="33"/>
-    </row>
-    <row r="26" spans="2:6" ht="15" x14ac:dyDescent="0.45">
+      <c r="C25" s="36" t="s">
+        <v>83</v>
+      </c>
+      <c r="D25" s="36"/>
+      <c r="E25" s="23">
+        <v>20</v>
+      </c>
+      <c r="F25" s="24" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B26" s="16"/>
-      <c r="C26" s="33"/>
-      <c r="D26" s="33"/>
-    </row>
-    <row r="27" spans="2:6" ht="15" x14ac:dyDescent="0.45">
+      <c r="C26" s="36" t="s">
+        <v>82</v>
+      </c>
+      <c r="D26" s="36"/>
+      <c r="E26" s="23">
+        <v>130</v>
+      </c>
+      <c r="F26" s="24" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B27" s="16"/>
-      <c r="C27" s="33"/>
-      <c r="D27" s="33"/>
-    </row>
-    <row r="28" spans="2:6" ht="15" x14ac:dyDescent="0.45">
+      <c r="C27" s="38" t="s">
+        <v>87</v>
+      </c>
+      <c r="D27" s="38"/>
+      <c r="E27" s="17">
+        <v>200</v>
+      </c>
+      <c r="F27" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="H27" s="34"/>
+    </row>
+    <row r="28" spans="2:8" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B28" s="16"/>
-      <c r="C28" s="33"/>
-      <c r="D28" s="33"/>
-    </row>
-    <row r="29" spans="2:6" ht="15" x14ac:dyDescent="0.45">
+      <c r="C28" s="37" t="s">
+        <v>81</v>
+      </c>
+      <c r="D28" s="37"/>
+      <c r="E28" s="21">
+        <v>200</v>
+      </c>
+      <c r="F28" s="22" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" ht="15" x14ac:dyDescent="0.45">
       <c r="B29" s="16"/>
-      <c r="C29" s="33"/>
-      <c r="D29" s="33"/>
-    </row>
-    <row r="30" spans="2:6" ht="15" x14ac:dyDescent="0.45">
+      <c r="C29" s="39"/>
+      <c r="D29" s="39"/>
+      <c r="F29" s="13"/>
+    </row>
+    <row r="30" spans="2:8" ht="15" x14ac:dyDescent="0.45">
       <c r="B30" s="16"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="33"/>
-    </row>
-    <row r="31" spans="2:6" ht="15" x14ac:dyDescent="0.45">
+      <c r="C30" s="39"/>
+      <c r="D30" s="39"/>
+    </row>
+    <row r="31" spans="2:8" ht="15" x14ac:dyDescent="0.45">
       <c r="B31" s="16"/>
-      <c r="C31" s="33"/>
-      <c r="D31" s="33"/>
-    </row>
-    <row r="32" spans="2:6" ht="15" x14ac:dyDescent="0.45">
+      <c r="C31" s="39"/>
+      <c r="D31" s="39"/>
+    </row>
+    <row r="32" spans="2:8" ht="15" x14ac:dyDescent="0.45">
       <c r="B32" s="16"/>
     </row>
     <row r="33" spans="2:2" ht="15" x14ac:dyDescent="0.45">
@@ -1461,26 +1604,26 @@
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="C14:D14"/>
     <mergeCell ref="C15:D15"/>
     <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C31:D31"/>
     <mergeCell ref="C22:D22"/>
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="C24:D24"/>
     <mergeCell ref="C25:D25"/>
     <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="C20:D20"/>
     <mergeCell ref="C27:D27"/>
     <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C31:D31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1510,10 +1653,10 @@
       <c r="B2" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="39" t="s">
+      <c r="C2" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="39"/>
+      <c r="D2" s="42"/>
       <c r="E2" s="8" t="s">
         <v>8</v>
       </c>
@@ -1528,10 +1671,10 @@
       <c r="B3" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="40" t="s">
+      <c r="C3" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="D3" s="40"/>
+      <c r="D3" s="43"/>
       <c r="E3" s="12" t="s">
         <v>29</v>
       </c>
@@ -1602,9 +1745,9 @@
       <c r="G11" s="4"/>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.45">
-      <c r="C12" s="33"/>
-      <c r="D12" s="33"/>
-      <c r="E12" s="33"/>
+      <c r="C12" s="39"/>
+      <c r="D12" s="39"/>
+      <c r="E12" s="39"/>
     </row>
     <row r="13" spans="2:7" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="8" t="s">
@@ -1743,10 +1886,10 @@
       <c r="B2" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="39" t="s">
+      <c r="C2" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="39"/>
+      <c r="D2" s="42"/>
       <c r="E2" s="10" t="s">
         <v>8</v>
       </c>
@@ -1761,10 +1904,10 @@
       <c r="B3" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="C3" s="40" t="s">
+      <c r="C3" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="40"/>
+      <c r="D3" s="43"/>
       <c r="E3" s="15" t="s">
         <v>29</v>
       </c>
@@ -2034,10 +2177,10 @@
       <c r="B2" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="39" t="s">
+      <c r="C2" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="39"/>
+      <c r="D2" s="42"/>
       <c r="E2" s="27" t="s">
         <v>8</v>
       </c>
@@ -2052,10 +2195,10 @@
       <c r="B3" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="C3" s="40" t="s">
+      <c r="C3" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="40"/>
+      <c r="D3" s="43"/>
       <c r="E3" s="28" t="s">
         <v>29</v>
       </c>
@@ -2330,10 +2473,10 @@
       <c r="B2" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="39" t="s">
+      <c r="C2" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="39"/>
+      <c r="D2" s="42"/>
       <c r="E2" s="29" t="s">
         <v>8</v>
       </c>
@@ -2348,10 +2491,10 @@
       <c r="B3" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="C3" s="40" t="s">
+      <c r="C3" s="43" t="s">
         <v>68</v>
       </c>
-      <c r="D3" s="40"/>
+      <c r="D3" s="43"/>
       <c r="E3" s="30" t="s">
         <v>29</v>
       </c>
@@ -2620,10 +2763,10 @@
       <c r="B2" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="39" t="s">
+      <c r="C2" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="39"/>
+      <c r="D2" s="42"/>
       <c r="E2" s="31" t="s">
         <v>8</v>
       </c>
@@ -2638,10 +2781,10 @@
       <c r="B3" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="40" t="s">
+      <c r="C3" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="D3" s="40"/>
+      <c r="D3" s="43"/>
       <c r="E3" s="32" t="s">
         <v>29</v>
       </c>
@@ -2918,8 +3061,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{654FEFB0-94AD-455F-A9BF-0EDC413A1355}">
   <dimension ref="B2:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView zoomScale="83" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2938,10 +3081,10 @@
       <c r="B2" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="39" t="s">
+      <c r="C2" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="39"/>
+      <c r="D2" s="42"/>
       <c r="E2" s="31" t="s">
         <v>8</v>
       </c>
@@ -2956,10 +3099,10 @@
       <c r="B3" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="C3" s="40" t="s">
+      <c r="C3" s="43" t="s">
         <v>75</v>
       </c>
-      <c r="D3" s="40"/>
+      <c r="D3" s="43"/>
       <c r="E3" s="32" t="s">
         <v>29</v>
       </c>
@@ -3217,6 +3360,512 @@
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
       <c r="G26" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D335EDD7-9A70-4917-918F-B8FBDAFF8061}">
+  <dimension ref="B2:G36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="83" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18:F28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="2.86328125" customWidth="1"/>
+    <col min="2" max="2" width="56.1328125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="34.265625" customWidth="1"/>
+    <col min="4" max="4" width="31.86328125" customWidth="1"/>
+    <col min="5" max="5" width="27" customWidth="1"/>
+    <col min="6" max="6" width="29.3984375" customWidth="1"/>
+    <col min="7" max="7" width="28.73046875" customWidth="1"/>
+    <col min="8" max="8" width="18.59765625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="42" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="42"/>
+      <c r="E2" s="33" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="33" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" s="14" customFormat="1" ht="21.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B3" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3" s="43" t="s">
+        <v>80</v>
+      </c>
+      <c r="D3" s="43"/>
+      <c r="E3" s="34" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="33" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="33" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" s="14" customFormat="1" ht="21.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B6" s="13"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+    </row>
+    <row r="7" spans="2:7" s="2" customFormat="1" ht="21.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B7" s="13"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+    </row>
+    <row r="9" spans="2:7" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="33" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" s="14" customFormat="1" ht="21.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B10" s="34" t="s">
+        <v>88</v>
+      </c>
+      <c r="C10" s="34">
+        <v>0</v>
+      </c>
+      <c r="D10" s="34">
+        <v>100</v>
+      </c>
+      <c r="E10" s="34">
+        <v>200</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" s="13" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" s="14" customFormat="1" ht="21.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B11" s="34" t="s">
+        <v>90</v>
+      </c>
+      <c r="C11" s="34">
+        <v>0</v>
+      </c>
+      <c r="D11" s="34">
+        <v>100</v>
+      </c>
+      <c r="E11" s="34">
+        <v>300</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" s="14" customFormat="1" ht="21.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B12" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="C12" s="34">
+        <v>0</v>
+      </c>
+      <c r="D12" s="34">
+        <v>100</v>
+      </c>
+      <c r="E12" s="34">
+        <v>50</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" s="14" customFormat="1" ht="21.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B13" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="C13" s="34">
+        <v>400</v>
+      </c>
+      <c r="D13" s="34">
+        <v>100</v>
+      </c>
+      <c r="E13" s="34">
+        <v>300</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" s="14" customFormat="1" ht="21.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B14" s="34" t="s">
+        <v>76</v>
+      </c>
+      <c r="C14" s="34">
+        <v>100</v>
+      </c>
+      <c r="D14" s="34">
+        <v>0</v>
+      </c>
+      <c r="E14" s="34">
+        <v>150</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" s="14" customFormat="1" ht="21.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B15" s="34"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="34"/>
+      <c r="E15" s="34"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+    </row>
+    <row r="17" spans="2:7" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" s="33" t="s">
+        <v>17</v>
+      </c>
+      <c r="F17" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="G17" s="33" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" s="14" customFormat="1" ht="21.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B18" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="C18" s="34">
+        <v>0</v>
+      </c>
+      <c r="D18" s="34">
+        <v>40</v>
+      </c>
+      <c r="E18" s="34">
+        <v>40</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="G18" s="34" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" s="14" customFormat="1" ht="21.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B19" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="C19" s="34">
+        <v>100</v>
+      </c>
+      <c r="D19" s="34">
+        <v>10</v>
+      </c>
+      <c r="E19" s="34">
+        <v>110</v>
+      </c>
+      <c r="F19" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="G19" s="34" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" s="14" customFormat="1" ht="21.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B20" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="C20" s="34">
+        <v>250</v>
+      </c>
+      <c r="D20" s="34">
+        <v>20</v>
+      </c>
+      <c r="E20" s="34">
+        <v>270</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="G20" s="34" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" s="14" customFormat="1" ht="21.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B21" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="C21" s="34">
+        <v>0</v>
+      </c>
+      <c r="D21" s="34">
+        <v>50</v>
+      </c>
+      <c r="E21" s="34">
+        <v>50</v>
+      </c>
+      <c r="F21" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="G21" s="34" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" s="14" customFormat="1" ht="21.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B22" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="C22" s="34">
+        <v>0</v>
+      </c>
+      <c r="D22" s="34">
+        <v>300</v>
+      </c>
+      <c r="E22" s="34">
+        <v>300</v>
+      </c>
+      <c r="F22" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="G22" s="34" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" s="14" customFormat="1" ht="21.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B23" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="C23" s="34">
+        <v>0</v>
+      </c>
+      <c r="D23" s="34">
+        <v>20</v>
+      </c>
+      <c r="E23" s="34">
+        <v>20</v>
+      </c>
+      <c r="F23" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="G23" s="34" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" s="14" customFormat="1" ht="21.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B24" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="C24" s="34">
+        <v>0</v>
+      </c>
+      <c r="D24" s="34">
+        <v>20</v>
+      </c>
+      <c r="E24" s="34">
+        <v>20</v>
+      </c>
+      <c r="F24" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="G24" s="34" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" s="14" customFormat="1" ht="21.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B25" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="C25" s="34">
+        <v>0</v>
+      </c>
+      <c r="D25" s="34">
+        <v>130</v>
+      </c>
+      <c r="E25" s="34">
+        <v>130</v>
+      </c>
+      <c r="F25" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="G25" s="34" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" s="14" customFormat="1" ht="21.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B26" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="C26" s="34">
+        <v>100</v>
+      </c>
+      <c r="D26" s="34">
+        <v>100</v>
+      </c>
+      <c r="E26" s="34">
+        <v>200</v>
+      </c>
+      <c r="F26" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="G26" s="34" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" s="14" customFormat="1" ht="21.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B27" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="C27" s="34">
+        <v>0</v>
+      </c>
+      <c r="D27" s="34">
+        <v>200</v>
+      </c>
+      <c r="E27" s="34">
+        <v>200</v>
+      </c>
+      <c r="F27" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="G27" s="34" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" s="14" customFormat="1" ht="21.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B28" s="13"/>
+      <c r="C28" s="34"/>
+      <c r="D28" s="34"/>
+      <c r="E28" s="34"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="34"/>
+    </row>
+    <row r="30" spans="2:7" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B30" s="33" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="D30" s="33" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" s="14" customFormat="1" ht="21.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B31" s="13"/>
+      <c r="C31" s="34"/>
+      <c r="D31" s="34"/>
+      <c r="E31" s="34"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
+    </row>
+    <row r="32" spans="2:7" s="14" customFormat="1" ht="21.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B32" s="13"/>
+      <c r="C32" s="34"/>
+      <c r="D32" s="34"/>
+      <c r="E32" s="34"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="13"/>
+    </row>
+    <row r="34" spans="2:7" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B34" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="C34" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="D34" s="33" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" s="14" customFormat="1" ht="21.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B35" s="7"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7"/>
+    </row>
+    <row r="36" spans="2:7" s="14" customFormat="1" ht="21.4" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="B36" s="7"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="7"/>
+      <c r="G36" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>